<commit_message>
sum of children property question solved
</commit_message>
<xml_diff>
--- a/DSA patterns Cheat Sheet.xlsx
+++ b/DSA patterns Cheat Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="370">
   <si>
     <t xml:space="preserve">INSTA Channel. One question Daily</t>
   </si>
@@ -1522,10 +1522,10 @@
   <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.35"/>
@@ -1583,7 +1583,9 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
@@ -1594,7 +1596,9 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1609,7 +1613,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
@@ -1620,7 +1626,9 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="B8" s="9" t="s">
         <v>18</v>
       </c>

</xml_diff>